<commit_message>
vault backup: 2024-04-24 14:21:37
</commit_message>
<xml_diff>
--- a/projects/quote-process-optimization/cwsell-quote-templates-modifications.xlsx
+++ b/projects/quote-process-optimization/cwsell-quote-templates-modifications.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meriplex-my.sharepoint.com/personal/ian_wheeler_meriplex_com/Documents/Documents/Obsidian/Meriplex/projects/quote-process-optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{11A91280-DB61-4019-9EC7-B3F316339DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72E1261F-117B-47B1-9286-BABBEFECF6DB}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{11A91280-DB61-4019-9EC7-B3F316339DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E81FC25A-0E44-4CAE-85BB-DBF6D4ABBB64}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="450" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6D55FE8F-C9AB-43F7-9348-63EA4D2256B3}"/>
+    <workbookView xWindow="28680" yWindow="450" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{6D55FE8F-C9AB-43F7-9348-63EA4D2256B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Group 1" sheetId="6" r:id="rId1"/>
     <sheet name="Group 2" sheetId="7" r:id="rId2"/>
+    <sheet name="Group 3" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="187">
   <si>
     <t>Description</t>
   </si>
@@ -575,13 +576,42 @@
   </si>
   <si>
     <t>Non-Recurring; copying over client details and signed information.</t>
+  </si>
+  <si>
+    <t>Michael True</t>
+  </si>
+  <si>
+    <t>Used for NRR Actual Rates Block of Hours
+Fixed hours block time
+Recommend merge with blended rates and consolidate products or add additional tab</t>
+  </si>
+  <si>
+    <t>Initially created by AM's for their specific needs.
+Recommend merge with actual rates and consolidate products or add additional tab
+Used for NRR Blended Rates Block of Hours</t>
+  </si>
+  <si>
+    <t>NRR Security Risk Assessment;
+Standardize the verbiage, and modify so the Order Porter, Grid Layout, and PDF reflect Meriplex standards.</t>
+  </si>
+  <si>
+    <t>Reach out to Mitch Verma to find out if these can be deprecated</t>
+  </si>
+  <si>
+    <t>SSI-NRR-Basic-Standard</t>
+  </si>
+  <si>
+    <t>SSI</t>
+  </si>
+  <si>
+    <t>Basic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -612,6 +642,14 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Aptos Narrow"/>
@@ -674,7 +712,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -694,65 +732,23 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -806,6 +802,46 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -840,21 +876,7 @@
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFEB9C"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -867,6 +889,20 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -896,10 +932,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C826E71F-1F09-4E74-AB87-A4B764A79312}" name="Table4" displayName="Table4" ref="A1:N116" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C826E71F-1F09-4E74-AB87-A4B764A79312}" name="Table4" displayName="Table4" ref="A1:N116" totalsRowShown="0" headerRowDxfId="31">
   <autoFilter ref="A1:N116" xr:uid="{C826E71F-1F09-4E74-AB87-A4B764A79312}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N116">
-    <sortCondition sortBy="cellColor" ref="A1:A116" dxfId="24"/>
+    <sortCondition sortBy="cellColor" ref="A1:A116" dxfId="30"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{1CDAD25C-2B9A-49A0-AF29-91C07A6E557F}" name="Quote Template Name"/>
@@ -908,24 +944,24 @@
     <tableColumn id="20" xr3:uid="{35674A47-F800-469A-8C5C-DD617AF44734}" name="Template Description"/>
     <tableColumn id="4" xr3:uid="{44A37B7D-BD53-4FF5-843D-F1B07DBB048A}" name="Type"/>
     <tableColumn id="22" xr3:uid="{6E558547-340A-49D0-8009-801D245C0CF2}" name="ModifiedBy"/>
-    <tableColumn id="7" xr3:uid="{78D4773A-F41A-4332-990A-390F054BF842}" name="Action" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{BA7416B4-3F5E-40EA-AD3C-257EA87B11DA}" name="Description" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{78D4773A-F41A-4332-990A-390F054BF842}" name="Action" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{BA7416B4-3F5E-40EA-AD3C-257EA87B11DA}" name="Description" dataDxfId="28"/>
     <tableColumn id="3" xr3:uid="{5EACD7CE-28E1-4D84-9371-73FEAE60A99A}" name="New Quote Template Name"/>
-    <tableColumn id="8" xr3:uid="{3E2DAFC4-4656-494A-8EBC-191A5A3B8CD9}" name="Notes" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{D425B706-2CE8-49E4-B19D-803E5519746B}" name="Jackie Moore" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{1A6DBD9C-5080-4FDB-AC9D-378744BB47DF}" name="Jerry Prestridge" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{917A0CCE-95BA-4484-B3CA-99D29C5F0E5D}" name="John Sobernheim" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{34C6A6A8-871B-46B7-8595-DD76FDE12BEA}" name="Laura Emery" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{3E2DAFC4-4656-494A-8EBC-191A5A3B8CD9}" name="Notes" dataDxfId="27"/>
+    <tableColumn id="11" xr3:uid="{D425B706-2CE8-49E4-B19D-803E5519746B}" name="Jackie Moore" dataDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{1A6DBD9C-5080-4FDB-AC9D-378744BB47DF}" name="Jerry Prestridge" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{917A0CCE-95BA-4484-B3CA-99D29C5F0E5D}" name="John Sobernheim" dataDxfId="24"/>
+    <tableColumn id="14" xr3:uid="{34C6A6A8-871B-46B7-8595-DD76FDE12BEA}" name="Laura Emery" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60CAD70A-275C-45C0-B731-B22CDDAE60F0}" name="Table43" displayName="Table43" ref="A1:O116" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60CAD70A-275C-45C0-B731-B22CDDAE60F0}" name="Table43" displayName="Table43" ref="A1:O116" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="A1:O116" xr:uid="{C826E71F-1F09-4E74-AB87-A4B764A79312}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O116">
-    <sortCondition sortBy="cellColor" ref="A1:A116" dxfId="19"/>
+    <sortCondition sortBy="cellColor" ref="A1:A116" dxfId="21"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{45394437-3E6A-4F3F-BF78-410AB14265B5}" name="Quote Template Name"/>
@@ -934,15 +970,40 @@
     <tableColumn id="20" xr3:uid="{0D9EF5A9-F9AE-4E35-A6F4-E02C4767597A}" name="Template Description"/>
     <tableColumn id="4" xr3:uid="{6A0C6F44-DE66-4399-8852-D40F5EC31B6D}" name="Type"/>
     <tableColumn id="22" xr3:uid="{ACE2F589-F42F-4677-AF87-597E2B3FB472}" name="ModifiedBy"/>
-    <tableColumn id="7" xr3:uid="{E679A7D9-4E17-42E3-A2AB-BF208BDFF899}" name="Action" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{9B74567D-748E-47C4-9942-2EECA3EFB23C}" name="Description" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{E679A7D9-4E17-42E3-A2AB-BF208BDFF899}" name="Action" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{9B74567D-748E-47C4-9942-2EECA3EFB23C}" name="Description" dataDxfId="19"/>
     <tableColumn id="3" xr3:uid="{16587333-4ECC-4E10-8149-3D9EFC0281FC}" name="New Quote Template Name"/>
-    <tableColumn id="8" xr3:uid="{2C2F549A-C90B-4728-89B5-8FD86E22B78D}" name="Notes" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{7FC7C08A-B805-418E-B672-9B5854AE4609}" name="Brian McShane" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{E1D34B11-E59C-4885-BC6E-B5ED745E6B41}" name="Cynthia Newsom" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{9FE09AE9-35EE-4245-AB90-A6180AEAE356}" name="Ron Walker" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{7D9F976A-122D-436E-9B15-145BAF9BE54B}" name="Shaun Kilkenny" dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{D1B3E339-E9A6-4E09-A665-C4CCB7A6D180}" name="Anthony Kazlauskas" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{2C2F549A-C90B-4728-89B5-8FD86E22B78D}" name="Notes" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{7FC7C08A-B805-418E-B672-9B5854AE4609}" name="Brian McShane" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{E1D34B11-E59C-4885-BC6E-B5ED745E6B41}" name="Cynthia Newsom" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{9FE09AE9-35EE-4245-AB90-A6180AEAE356}" name="Ron Walker" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{7D9F976A-122D-436E-9B15-145BAF9BE54B}" name="Shaun Kilkenny" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{D1B3E339-E9A6-4E09-A665-C4CCB7A6D180}" name="Anthony Kazlauskas" dataDxfId="13"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77D5C09C-E48B-49E3-91D3-B1F94796B377}" name="Table432" displayName="Table432" ref="A1:M117" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="A1:M117" xr:uid="{C826E71F-1F09-4E74-AB87-A4B764A79312}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M117">
+    <sortCondition sortBy="cellColor" ref="A1:A117" dxfId="11"/>
+  </sortState>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{35E26AB3-7DB7-4BA1-AE09-912A617DAC46}" name="Quote Template Name"/>
+    <tableColumn id="19" xr3:uid="{E897A686-9B5F-4020-90AA-05C8A4B3F6CA}" name="Company ID"/>
+    <tableColumn id="21" xr3:uid="{63FE4D86-2BC1-4DD2-85D2-D0CC93EA165D}" name="Category"/>
+    <tableColumn id="20" xr3:uid="{707287BE-86D8-45D0-88DD-EBBE0D20BD8E}" name="Template Description"/>
+    <tableColumn id="4" xr3:uid="{F5251A50-E6EB-4E27-8184-A42E9DFCAB57}" name="Type"/>
+    <tableColumn id="22" xr3:uid="{EECB5098-35C9-4AD9-B6AE-52E90C0CBCF0}" name="ModifiedBy"/>
+    <tableColumn id="7" xr3:uid="{BA393A1F-2D2D-4D84-8BFE-099153C6F9F4}" name="Action" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{CCC4ED4F-86BD-4025-BC11-77138AFC29BD}" name="Description" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{67FE4F5D-40AE-4DBE-9858-CFBA67BD4D7A}" name="New Quote Template Name"/>
+    <tableColumn id="8" xr3:uid="{E2F74654-1683-4BD2-A3F4-D6F09C39CD23}" name="Notes" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{72B88A1B-5DA2-4C1F-9AD2-63FCE71F3608}" name="Michael True" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{2BF86793-478E-46BB-A90C-0AC8AD235068}" name="Shaun Kilkenny" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{58A4C243-A29A-4937-8ACA-5B85B31E2CFA}" name="Anthony Kazlauskas" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1283,7 +1344,7 @@
     <col min="8" max="8" width="102" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="58.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="102" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -1321,7 +1382,7 @@
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -1363,14 +1424,14 @@
       <c r="G2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>159</v>
       </c>
       <c r="I2" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Block of Hours - Actual Rates]-STANDARD</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K2" s="5"/>
@@ -1398,14 +1459,14 @@
       <c r="G3" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>133</v>
       </c>
       <c r="I3" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Block of Hours - Blended Rates]-STANDARD</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>133</v>
       </c>
       <c r="K3" s="5"/>
@@ -1427,14 +1488,14 @@
       <c r="G4" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="7" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="8"/>
@@ -1462,14 +1523,14 @@
       <c r="G5" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>136</v>
       </c>
       <c r="I5" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Time &amp; Materials]-STANDARD</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>136</v>
       </c>
       <c r="K5" s="5"/>
@@ -1499,14 +1560,14 @@
       <c r="G6" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>139</v>
       </c>
       <c r="I6" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Upfront (Annual)]-STANDARD</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>139</v>
       </c>
       <c r="K6" s="5" t="s">
@@ -1538,14 +1599,14 @@
       <c r="G7" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-HYBRID-[Change Order]-STANDARD</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -1579,14 +1640,14 @@
       <c r="G8" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>140</v>
       </c>
       <c r="I8" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[GCC High Licenses - Add On Orders]-STANDARD</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>140</v>
       </c>
       <c r="K8" s="5"/>
@@ -1616,14 +1677,14 @@
       <c r="G9" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I9" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[GCC High Licenses - Contract Addendum]-STANDARD</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="9" t="s">
         <v>141</v>
       </c>
       <c r="K9" s="5"/>
@@ -1653,14 +1714,14 @@
       <c r="G10" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>163</v>
       </c>
       <c r="I10" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Block of Hours - Actual Rates]-STANDARD</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>143</v>
       </c>
       <c r="K10" s="5"/>
@@ -1692,14 +1753,14 @@
       <c r="G11" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>142</v>
       </c>
       <c r="I11" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Block of Hours - Blended Rates]-STANDARD</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K11" s="5"/>
@@ -1731,14 +1792,14 @@
       <c r="G12" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>147</v>
       </c>
       <c r="I12" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Non-Recurring]-STANDARD</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="9" t="s">
         <v>147</v>
       </c>
       <c r="K12" s="5"/>
@@ -1770,14 +1831,14 @@
       <c r="G13" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>148</v>
       </c>
       <c r="I13" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Non-Recurring - Legacy Bronze]-STANDARD</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>148</v>
       </c>
       <c r="K13" s="5"/>
@@ -1809,14 +1870,14 @@
       <c r="G14" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>150</v>
       </c>
       <c r="I14" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Renewal]-STANDARD</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="9" t="s">
         <v>150</v>
       </c>
       <c r="K14" s="5"/>
@@ -1838,12 +1899,12 @@
       <c r="G15" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H15" s="11"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="7" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J15" s="11"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
@@ -1861,12 +1922,12 @@
       <c r="G16" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H16" s="10"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J16" s="10"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
@@ -1884,12 +1945,12 @@
       <c r="G17" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="7" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J17" s="11"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -1913,14 +1974,14 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Non-Recurring]-STANDARD</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="9" t="s">
         <v>25</v>
       </c>
       <c r="K18" s="5" t="s">
@@ -1946,12 +2007,12 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="10"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J19" s="10"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
@@ -1975,14 +2036,14 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>151</v>
       </c>
       <c r="I20" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[OHD Master Quotes]-CLIENT</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="9" t="s">
         <v>151</v>
       </c>
       <c r="K20" s="5" t="s">
@@ -2012,14 +2073,14 @@
       <c r="G21" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
         <v>144</v>
       </c>
       <c r="I21" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Physical Security]-STANDARD</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="9" t="s">
         <v>144</v>
       </c>
       <c r="K21" s="5" t="s">
@@ -2051,14 +2112,14 @@
       <c r="G22" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="9" t="s">
         <v>154</v>
       </c>
       <c r="I22" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Firewall End of Service Renewal]-USER-JSobernheim</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="9" t="s">
         <v>154</v>
       </c>
       <c r="K22" s="5"/>
@@ -2078,12 +2139,12 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="11"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="7" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="10"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
@@ -2109,14 +2170,14 @@
       <c r="G24" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>155</v>
       </c>
       <c r="I24" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Renewal]-STANDARD</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="9" t="s">
         <v>155</v>
       </c>
       <c r="K24" s="5" t="s">
@@ -2148,14 +2209,14 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>156</v>
       </c>
       <c r="I25" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>RIT-NRR-[Security Risk Assessment]-STANDARD</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="9" t="s">
         <v>156</v>
       </c>
       <c r="K25" s="5"/>
@@ -2179,12 +2240,12 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="10"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>VMS-NRR-[Fixed Labor Rates]-</v>
       </c>
-      <c r="J26" s="10"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
@@ -2206,12 +2267,12 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="10"/>
+      <c r="H27" s="9"/>
       <c r="I27" s="1" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>VMS-NRR-[PSP Labor Rates]-</v>
       </c>
-      <c r="J27" s="10"/>
+      <c r="J27" s="9"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
@@ -2235,12 +2296,12 @@
       <c r="G28" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H28" s="11"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="7" t="str">
         <f>_xlfn.CONCAT(Table4[[#This Row],[Company ID]], "-", Table4[[#This Row],[Category]], "-[", Table4[[#This Row],[Template Description]], "]-", IF(Table4[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table4[[#This Row],[Type]], "-", Table4[[#This Row],[ModifiedBy]]), Table4[[#This Row],[Type]]))</f>
         <v>VMS-NRR-[Renewal]-</v>
       </c>
-      <c r="J28" s="11"/>
+      <c r="J28" s="10"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
@@ -2251,7 +2312,6 @@
         <v>36</v>
       </c>
       <c r="G29" s="6"/>
-      <c r="H29" s="12"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -2262,7 +2322,6 @@
         <v>38</v>
       </c>
       <c r="G30" s="6"/>
-      <c r="H30" s="12"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
@@ -2273,7 +2332,7 @@
         <v>39</v>
       </c>
       <c r="G31" s="6"/>
-      <c r="H31" s="12" t="s">
+      <c r="H31" t="s">
         <v>135</v>
       </c>
       <c r="K31" s="6"/>
@@ -2286,7 +2345,6 @@
         <v>40</v>
       </c>
       <c r="G32" s="6"/>
-      <c r="H32" s="12"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
@@ -2297,7 +2355,7 @@
         <v>41</v>
       </c>
       <c r="G33" s="6"/>
-      <c r="H33" s="12" t="s">
+      <c r="H33" t="s">
         <v>126</v>
       </c>
       <c r="K33" s="6"/>
@@ -2310,7 +2368,6 @@
         <v>42</v>
       </c>
       <c r="G34" s="6"/>
-      <c r="H34" s="12"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
@@ -2321,7 +2378,7 @@
         <v>43</v>
       </c>
       <c r="G35" s="6"/>
-      <c r="H35" s="12" t="s">
+      <c r="H35" t="s">
         <v>158</v>
       </c>
       <c r="K35" s="6"/>
@@ -2334,7 +2391,7 @@
         <v>44</v>
       </c>
       <c r="G36" s="6"/>
-      <c r="H36" s="12" t="s">
+      <c r="H36" t="s">
         <v>158</v>
       </c>
       <c r="K36" s="6"/>
@@ -2347,7 +2404,7 @@
         <v>45</v>
       </c>
       <c r="G37" s="6"/>
-      <c r="H37" s="12" t="s">
+      <c r="H37" t="s">
         <v>158</v>
       </c>
       <c r="K37" s="6"/>
@@ -2360,7 +2417,7 @@
         <v>46</v>
       </c>
       <c r="G38" s="6"/>
-      <c r="H38" s="12" t="s">
+      <c r="H38" t="s">
         <v>158</v>
       </c>
       <c r="K38" s="6"/>
@@ -2373,7 +2430,7 @@
         <v>47</v>
       </c>
       <c r="G39" s="6"/>
-      <c r="H39" s="12" t="s">
+      <c r="H39" t="s">
         <v>158</v>
       </c>
       <c r="K39" s="6"/>
@@ -2386,7 +2443,7 @@
         <v>48</v>
       </c>
       <c r="G40" s="6"/>
-      <c r="H40" s="12" t="s">
+      <c r="H40" t="s">
         <v>158</v>
       </c>
       <c r="K40" s="6"/>
@@ -2399,7 +2456,7 @@
         <v>49</v>
       </c>
       <c r="G41" s="6"/>
-      <c r="H41" s="12" t="s">
+      <c r="H41" t="s">
         <v>158</v>
       </c>
       <c r="K41" s="6"/>
@@ -2412,7 +2469,7 @@
         <v>50</v>
       </c>
       <c r="G42" s="6"/>
-      <c r="H42" s="12" t="s">
+      <c r="H42" t="s">
         <v>149</v>
       </c>
       <c r="K42" s="6"/>
@@ -2425,7 +2482,6 @@
         <v>51</v>
       </c>
       <c r="G43" s="6"/>
-      <c r="H43" s="12"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
@@ -2436,7 +2492,6 @@
         <v>52</v>
       </c>
       <c r="G44" s="6"/>
-      <c r="H44" s="12"/>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
@@ -2447,7 +2502,6 @@
         <v>53</v>
       </c>
       <c r="G45" s="6"/>
-      <c r="H45" s="12"/>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
@@ -2458,7 +2512,6 @@
         <v>54</v>
       </c>
       <c r="G46" s="6"/>
-      <c r="H46" s="12"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
@@ -2469,7 +2522,6 @@
         <v>55</v>
       </c>
       <c r="G47" s="6"/>
-      <c r="H47" s="12"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
@@ -2480,7 +2532,7 @@
         <v>56</v>
       </c>
       <c r="G48" s="6"/>
-      <c r="H48" s="12" t="s">
+      <c r="H48" t="s">
         <v>153</v>
       </c>
       <c r="K48" s="6"/>
@@ -2493,7 +2545,6 @@
         <v>57</v>
       </c>
       <c r="G49" s="6"/>
-      <c r="H49" s="12"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
@@ -2504,7 +2555,6 @@
         <v>58</v>
       </c>
       <c r="G50" s="6"/>
-      <c r="H50" s="12"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
@@ -2515,7 +2565,6 @@
         <v>59</v>
       </c>
       <c r="G51" s="6"/>
-      <c r="H51" s="12"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
@@ -2526,7 +2575,6 @@
         <v>60</v>
       </c>
       <c r="G52" s="6"/>
-      <c r="H52" s="12"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
@@ -2537,7 +2585,6 @@
         <v>61</v>
       </c>
       <c r="G53" s="6"/>
-      <c r="H53" s="12"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
@@ -2548,7 +2595,6 @@
         <v>62</v>
       </c>
       <c r="G54" s="6"/>
-      <c r="H54" s="12"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
@@ -2559,7 +2605,6 @@
         <v>63</v>
       </c>
       <c r="G55" s="6"/>
-      <c r="H55" s="12"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
@@ -2575,7 +2620,7 @@
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="11"/>
+      <c r="H56" s="10"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="8"/>
@@ -2595,7 +2640,7 @@
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="11"/>
+      <c r="H57" s="10"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="8"/>
@@ -2615,7 +2660,7 @@
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="11"/>
+      <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="8"/>
@@ -2635,7 +2680,7 @@
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="11"/>
+      <c r="H59" s="10"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="8"/>
@@ -2655,7 +2700,7 @@
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="11"/>
+      <c r="H60" s="10"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="8"/>
@@ -2670,7 +2715,6 @@
         <v>64</v>
       </c>
       <c r="G61" s="6"/>
-      <c r="H61" s="12"/>
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
       <c r="M61" s="6"/>
@@ -2681,7 +2725,6 @@
         <v>65</v>
       </c>
       <c r="G62" s="6"/>
-      <c r="H62" s="12"/>
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
@@ -2692,7 +2735,6 @@
         <v>66</v>
       </c>
       <c r="G63" s="6"/>
-      <c r="H63" s="12"/>
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
       <c r="M63" s="6"/>
@@ -2703,7 +2745,6 @@
         <v>67</v>
       </c>
       <c r="G64" s="6"/>
-      <c r="H64" s="12"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
       <c r="M64" s="6"/>
@@ -2714,7 +2755,6 @@
         <v>68</v>
       </c>
       <c r="G65" s="6"/>
-      <c r="H65" s="12"/>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
@@ -2725,7 +2765,6 @@
         <v>69</v>
       </c>
       <c r="G66" s="6"/>
-      <c r="H66" s="12"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
@@ -2736,7 +2775,6 @@
         <v>70</v>
       </c>
       <c r="G67" s="6"/>
-      <c r="H67" s="12"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
@@ -2747,7 +2785,6 @@
         <v>71</v>
       </c>
       <c r="G68" s="6"/>
-      <c r="H68" s="12"/>
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
       <c r="M68" s="6"/>
@@ -2758,7 +2795,6 @@
         <v>72</v>
       </c>
       <c r="G69" s="6"/>
-      <c r="H69" s="12"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="6"/>
@@ -2769,7 +2805,6 @@
         <v>73</v>
       </c>
       <c r="G70" s="6"/>
-      <c r="H70" s="12"/>
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
       <c r="M70" s="6"/>
@@ -2780,7 +2815,6 @@
         <v>74</v>
       </c>
       <c r="G71" s="6"/>
-      <c r="H71" s="12"/>
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
       <c r="M71" s="6"/>
@@ -2791,7 +2825,6 @@
         <v>75</v>
       </c>
       <c r="G72" s="6"/>
-      <c r="H72" s="12"/>
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
       <c r="M72" s="6"/>
@@ -2802,7 +2835,6 @@
         <v>76</v>
       </c>
       <c r="G73" s="6"/>
-      <c r="H73" s="12"/>
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
       <c r="M73" s="6"/>
@@ -2813,7 +2845,6 @@
         <v>77</v>
       </c>
       <c r="G74" s="6"/>
-      <c r="H74" s="12"/>
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
       <c r="M74" s="6"/>
@@ -2824,7 +2855,6 @@
         <v>78</v>
       </c>
       <c r="G75" s="6"/>
-      <c r="H75" s="12"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
@@ -2835,7 +2865,6 @@
         <v>79</v>
       </c>
       <c r="G76" s="6"/>
-      <c r="H76" s="12"/>
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
       <c r="M76" s="6"/>
@@ -2846,7 +2875,6 @@
         <v>80</v>
       </c>
       <c r="G77" s="6"/>
-      <c r="H77" s="12"/>
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
       <c r="M77" s="6"/>
@@ -2857,7 +2885,6 @@
         <v>81</v>
       </c>
       <c r="G78" s="6"/>
-      <c r="H78" s="12"/>
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
       <c r="M78" s="6"/>
@@ -2868,7 +2895,6 @@
         <v>82</v>
       </c>
       <c r="G79" s="6"/>
-      <c r="H79" s="12"/>
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
       <c r="M79" s="6"/>
@@ -2879,7 +2905,6 @@
         <v>83</v>
       </c>
       <c r="G80" s="6"/>
-      <c r="H80" s="12"/>
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
       <c r="M80" s="6"/>
@@ -2890,7 +2915,6 @@
         <v>84</v>
       </c>
       <c r="G81" s="6"/>
-      <c r="H81" s="12"/>
       <c r="K81" s="6"/>
       <c r="L81" s="6"/>
       <c r="M81" s="6"/>
@@ -2901,7 +2925,6 @@
         <v>85</v>
       </c>
       <c r="G82" s="6"/>
-      <c r="H82" s="12"/>
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
       <c r="M82" s="6"/>
@@ -2912,7 +2935,6 @@
         <v>85</v>
       </c>
       <c r="G83" s="6"/>
-      <c r="H83" s="12"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
       <c r="M83" s="6"/>
@@ -2923,7 +2945,6 @@
         <v>86</v>
       </c>
       <c r="G84" s="6"/>
-      <c r="H84" s="12"/>
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
       <c r="M84" s="6"/>
@@ -2934,7 +2955,6 @@
         <v>87</v>
       </c>
       <c r="G85" s="6"/>
-      <c r="H85" s="12"/>
       <c r="K85" s="6"/>
       <c r="L85" s="6"/>
       <c r="M85" s="6"/>
@@ -2945,7 +2965,6 @@
         <v>88</v>
       </c>
       <c r="G86" s="6"/>
-      <c r="H86" s="12"/>
       <c r="K86" s="6"/>
       <c r="L86" s="6"/>
       <c r="M86" s="6"/>
@@ -2956,7 +2975,6 @@
         <v>89</v>
       </c>
       <c r="G87" s="6"/>
-      <c r="H87" s="12"/>
       <c r="K87" s="6"/>
       <c r="L87" s="6"/>
       <c r="M87" s="6"/>
@@ -2967,7 +2985,6 @@
         <v>90</v>
       </c>
       <c r="G88" s="6"/>
-      <c r="H88" s="12"/>
       <c r="K88" s="6"/>
       <c r="L88" s="6"/>
       <c r="M88" s="6"/>
@@ -2978,7 +2995,6 @@
         <v>91</v>
       </c>
       <c r="G89" s="6"/>
-      <c r="H89" s="12"/>
       <c r="K89" s="6"/>
       <c r="L89" s="6"/>
       <c r="M89" s="6"/>
@@ -2989,7 +3005,6 @@
         <v>92</v>
       </c>
       <c r="G90" s="6"/>
-      <c r="H90" s="12"/>
       <c r="K90" s="6"/>
       <c r="L90" s="6"/>
       <c r="M90" s="6"/>
@@ -3000,7 +3015,6 @@
         <v>93</v>
       </c>
       <c r="G91" s="6"/>
-      <c r="H91" s="12"/>
       <c r="K91" s="6"/>
       <c r="L91" s="6"/>
       <c r="M91" s="6"/>
@@ -3011,7 +3025,6 @@
         <v>94</v>
       </c>
       <c r="G92" s="6"/>
-      <c r="H92" s="12"/>
       <c r="K92" s="6"/>
       <c r="L92" s="6"/>
       <c r="M92" s="6"/>
@@ -3022,7 +3035,6 @@
         <v>95</v>
       </c>
       <c r="G93" s="6"/>
-      <c r="H93" s="12"/>
       <c r="K93" s="6"/>
       <c r="L93" s="6"/>
       <c r="M93" s="6"/>
@@ -3033,7 +3045,6 @@
         <v>96</v>
       </c>
       <c r="G94" s="6"/>
-      <c r="H94" s="12"/>
       <c r="K94" s="6"/>
       <c r="L94" s="6"/>
       <c r="M94" s="6"/>
@@ -3044,7 +3055,6 @@
         <v>97</v>
       </c>
       <c r="G95" s="6"/>
-      <c r="H95" s="12"/>
       <c r="K95" s="6"/>
       <c r="L95" s="6"/>
       <c r="M95" s="6"/>
@@ -3055,7 +3065,6 @@
         <v>97</v>
       </c>
       <c r="G96" s="6"/>
-      <c r="H96" s="12"/>
       <c r="K96" s="6"/>
       <c r="L96" s="6"/>
       <c r="M96" s="6"/>
@@ -3066,7 +3075,6 @@
         <v>97</v>
       </c>
       <c r="G97" s="6"/>
-      <c r="H97" s="12"/>
       <c r="K97" s="6"/>
       <c r="L97" s="6"/>
       <c r="M97" s="6"/>
@@ -3077,7 +3085,6 @@
         <v>98</v>
       </c>
       <c r="G98" s="6"/>
-      <c r="H98" s="12"/>
       <c r="K98" s="6"/>
       <c r="L98" s="6"/>
       <c r="M98" s="6"/>
@@ -3088,7 +3095,6 @@
         <v>99</v>
       </c>
       <c r="G99" s="6"/>
-      <c r="H99" s="12"/>
       <c r="K99" s="6"/>
       <c r="L99" s="6"/>
       <c r="M99" s="6"/>
@@ -3099,7 +3105,6 @@
         <v>100</v>
       </c>
       <c r="G100" s="6"/>
-      <c r="H100" s="12"/>
       <c r="K100" s="6"/>
       <c r="L100" s="6"/>
       <c r="M100" s="6"/>
@@ -3110,7 +3115,6 @@
         <v>101</v>
       </c>
       <c r="G101" s="6"/>
-      <c r="H101" s="12"/>
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
       <c r="M101" s="6"/>
@@ -3121,7 +3125,6 @@
         <v>102</v>
       </c>
       <c r="G102" s="6"/>
-      <c r="H102" s="12"/>
       <c r="K102" s="6"/>
       <c r="L102" s="6"/>
       <c r="M102" s="6"/>
@@ -3132,7 +3135,6 @@
         <v>103</v>
       </c>
       <c r="G103" s="6"/>
-      <c r="H103" s="12"/>
       <c r="K103" s="6"/>
       <c r="L103" s="6"/>
       <c r="M103" s="6"/>
@@ -3143,7 +3145,6 @@
         <v>104</v>
       </c>
       <c r="G104" s="6"/>
-      <c r="H104" s="12"/>
       <c r="K104" s="6"/>
       <c r="L104" s="6"/>
       <c r="M104" s="6"/>
@@ -3154,7 +3155,6 @@
         <v>105</v>
       </c>
       <c r="G105" s="6"/>
-      <c r="H105" s="12"/>
       <c r="K105" s="6"/>
       <c r="L105" s="6"/>
       <c r="M105" s="6"/>
@@ -3165,7 +3165,6 @@
         <v>106</v>
       </c>
       <c r="G106" s="6"/>
-      <c r="H106" s="12"/>
       <c r="K106" s="6"/>
       <c r="L106" s="6"/>
       <c r="M106" s="6"/>
@@ -3176,7 +3175,6 @@
         <v>107</v>
       </c>
       <c r="G107" s="6"/>
-      <c r="H107" s="12"/>
       <c r="K107" s="6"/>
       <c r="L107" s="6"/>
       <c r="M107" s="6"/>
@@ -3187,7 +3185,6 @@
         <v>108</v>
       </c>
       <c r="G108" s="6"/>
-      <c r="H108" s="12"/>
       <c r="K108" s="6"/>
       <c r="L108" s="6"/>
       <c r="M108" s="6"/>
@@ -3198,7 +3195,6 @@
         <v>109</v>
       </c>
       <c r="G109" s="6"/>
-      <c r="H109" s="12"/>
       <c r="K109" s="6"/>
       <c r="L109" s="6"/>
       <c r="M109" s="6"/>
@@ -3209,7 +3205,6 @@
         <v>110</v>
       </c>
       <c r="G110" s="6"/>
-      <c r="H110" s="12"/>
       <c r="K110" s="6"/>
       <c r="L110" s="6"/>
       <c r="M110" s="6"/>
@@ -3220,7 +3215,6 @@
         <v>111</v>
       </c>
       <c r="G111" s="6"/>
-      <c r="H111" s="12"/>
       <c r="K111" s="6"/>
       <c r="L111" s="6"/>
       <c r="M111" s="6"/>
@@ -3231,7 +3225,6 @@
         <v>112</v>
       </c>
       <c r="G112" s="6"/>
-      <c r="H112" s="12"/>
       <c r="K112" s="6"/>
       <c r="L112" s="6"/>
       <c r="M112" s="6"/>
@@ -3242,7 +3235,6 @@
         <v>113</v>
       </c>
       <c r="G113" s="6"/>
-      <c r="H113" s="12"/>
       <c r="K113" s="6"/>
       <c r="L113" s="6"/>
       <c r="M113" s="6"/>
@@ -3253,7 +3245,6 @@
         <v>114</v>
       </c>
       <c r="G114" s="6"/>
-      <c r="H114" s="12"/>
       <c r="K114" s="6"/>
       <c r="L114" s="6"/>
       <c r="M114" s="6"/>
@@ -3264,7 +3255,6 @@
         <v>115</v>
       </c>
       <c r="G115" s="6"/>
-      <c r="H115" s="12"/>
       <c r="K115" s="6"/>
       <c r="L115" s="6"/>
       <c r="M115" s="6"/>
@@ -3275,7 +3265,6 @@
         <v>116</v>
       </c>
       <c r="G116" s="6"/>
-      <c r="H116" s="12"/>
       <c r="K116" s="6"/>
       <c r="L116" s="6"/>
       <c r="M116" s="6"/>
@@ -3308,8 +3297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EE184F-A1E5-4A2B-B551-77C3606D37CA}">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3362,7 +3351,7 @@
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -3407,14 +3396,14 @@
       <c r="G2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>159</v>
       </c>
       <c r="I2" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Block of Hours - Actual Rates]-STANDARD</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>159</v>
       </c>
       <c r="K2" s="5" t="s">
@@ -3445,14 +3434,14 @@
       <c r="G3" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>133</v>
       </c>
       <c r="I3" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Block of Hours - Blended Rates]-STANDARD</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>133</v>
       </c>
       <c r="K3" s="5" t="s">
@@ -3479,14 +3468,14 @@
       <c r="G4" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="7" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="8" t="s">
@@ -3521,14 +3510,14 @@
       <c r="G5" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>136</v>
       </c>
       <c r="I5" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Time &amp; Materials]-STANDARD</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>136</v>
       </c>
       <c r="K5" s="5" t="s">
@@ -3561,14 +3550,14 @@
       <c r="G6" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>139</v>
       </c>
       <c r="I6" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Upfront (Annual)]-STANDARD</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>139</v>
       </c>
       <c r="K6" s="5" t="s">
@@ -3599,14 +3588,14 @@
       <c r="G7" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-HYBRID-[Change Order]-STANDARD</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K7" s="5" t="s">
@@ -3641,14 +3630,14 @@
       <c r="G8" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>140</v>
       </c>
       <c r="I8" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[GCC High Licenses - Add On Orders]-STANDARD</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>140</v>
       </c>
       <c r="K8" s="5" t="s">
@@ -3679,14 +3668,14 @@
       <c r="G9" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>141</v>
       </c>
       <c r="I9" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[GCC High Licenses - Contract Addendum]-STANDARD</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="9" t="s">
         <v>141</v>
       </c>
       <c r="K9" s="5" t="s">
@@ -3717,14 +3706,14 @@
       <c r="G10" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>163</v>
       </c>
       <c r="I10" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Block of Hours - Actual Rates]-STANDARD</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>143</v>
       </c>
       <c r="K10" s="5" t="s">
@@ -3755,14 +3744,14 @@
       <c r="G11" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>142</v>
       </c>
       <c r="I11" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Block of Hours - Blended Rates]-STANDARD</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="9" t="s">
         <v>142</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -3793,14 +3782,14 @@
       <c r="G12" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>147</v>
       </c>
       <c r="I12" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Non-Recurring]-STANDARD</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="9" t="s">
         <v>147</v>
       </c>
       <c r="K12" s="5" t="s">
@@ -3831,14 +3820,14 @@
       <c r="G13" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>148</v>
       </c>
       <c r="I13" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Non-Recurring - Legacy Bronze]-STANDARD</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>148</v>
       </c>
       <c r="K13" s="5" t="s">
@@ -3869,14 +3858,14 @@
       <c r="G14" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>150</v>
       </c>
       <c r="I14" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>GOV-NRR-[Renewal]-STANDARD</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="9" t="s">
         <v>150</v>
       </c>
       <c r="K14" s="5" t="s">
@@ -3899,12 +3888,12 @@
       <c r="G15" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H15" s="11"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="7" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J15" s="11"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="8" t="s">
         <v>128</v>
       </c>
@@ -3925,12 +3914,12 @@
       <c r="G16" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H16" s="10"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J16" s="10"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="5" t="s">
         <v>128</v>
       </c>
@@ -3951,12 +3940,12 @@
       <c r="G17" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="7" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J17" s="11"/>
+      <c r="J17" s="10"/>
       <c r="K17" s="8" t="s">
         <v>128</v>
       </c>
@@ -3985,14 +3974,14 @@
       <c r="G18" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>178</v>
       </c>
       <c r="I18" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Non-Recurring]-STANDARD</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="9" t="s">
         <v>25</v>
       </c>
       <c r="K18" s="5" t="s">
@@ -4014,12 +4003,12 @@
       <c r="G19" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H19" s="11"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="7" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="10"/>
       <c r="K19" s="8" t="s">
         <v>128</v>
       </c>
@@ -4048,14 +4037,14 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="9" t="s">
         <v>151</v>
       </c>
       <c r="I20" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[OHD Master Quotes]-CLIENT</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="9" t="s">
         <v>151</v>
       </c>
       <c r="K20" s="5" t="s">
@@ -4086,14 +4075,14 @@
       <c r="G21" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="9" t="s">
         <v>144</v>
       </c>
       <c r="I21" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Physical Security]-STANDARD</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="9" t="s">
         <v>144</v>
       </c>
       <c r="K21" s="5" t="s">
@@ -4126,14 +4115,14 @@
       <c r="G22" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="9" t="s">
         <v>154</v>
       </c>
       <c r="I22" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Firewall End of Service Renewal]-USER-JSobernheim</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="9" t="s">
         <v>154</v>
       </c>
       <c r="K22" s="5" t="s">
@@ -4154,12 +4143,12 @@
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="11"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="7" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>--[]-</v>
       </c>
-      <c r="J23" s="11"/>
+      <c r="J23" s="10"/>
       <c r="K23" s="8" t="s">
         <v>128</v>
       </c>
@@ -4188,14 +4177,14 @@
       <c r="G24" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="9" t="s">
         <v>155</v>
       </c>
       <c r="I24" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>MPC-NRR-[Renewal]-STANDARD</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" s="9" t="s">
         <v>155</v>
       </c>
       <c r="K24" s="5" t="s">
@@ -4224,14 +4213,14 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="10" t="s">
+      <c r="H25" s="9" t="s">
         <v>156</v>
       </c>
       <c r="I25" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>RIT-NRR-[Security Risk Assessment]-STANDARD</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" s="9" t="s">
         <v>156</v>
       </c>
       <c r="K25" s="5" t="s">
@@ -4258,12 +4247,12 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="10"/>
+      <c r="H26" s="9"/>
       <c r="I26" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>VMS-NRR-[Fixed Labor Rates]-</v>
       </c>
-      <c r="J26" s="10"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="5" t="s">
         <v>128</v>
       </c>
@@ -4288,12 +4277,12 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="10"/>
+      <c r="H27" s="9"/>
       <c r="I27" s="1" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>VMS-NRR-[PSP Labor Rates]-</v>
       </c>
-      <c r="J27" s="10"/>
+      <c r="J27" s="9"/>
       <c r="K27" s="5" t="s">
         <v>128</v>
       </c>
@@ -4320,12 +4309,12 @@
       <c r="G28" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H28" s="11"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="7" t="str">
         <f>_xlfn.CONCAT(Table43[[#This Row],[Company ID]], "-", Table43[[#This Row],[Category]], "-[", Table43[[#This Row],[Template Description]], "]-", IF(Table43[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table43[[#This Row],[Type]], "-", Table43[[#This Row],[ModifiedBy]]), Table43[[#This Row],[Type]]))</f>
         <v>VMS-NRR-[Renewal]-</v>
       </c>
-      <c r="J28" s="11"/>
+      <c r="J28" s="10"/>
       <c r="K28" s="8" t="s">
         <v>128</v>
       </c>
@@ -4339,7 +4328,6 @@
         <v>36</v>
       </c>
       <c r="G29" s="6"/>
-      <c r="H29" s="12"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -4351,7 +4339,6 @@
         <v>38</v>
       </c>
       <c r="G30" s="6"/>
-      <c r="H30" s="12"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
@@ -4363,7 +4350,7 @@
         <v>39</v>
       </c>
       <c r="G31" s="6"/>
-      <c r="H31" s="12" t="s">
+      <c r="H31" t="s">
         <v>135</v>
       </c>
       <c r="K31" s="6"/>
@@ -4377,7 +4364,6 @@
         <v>40</v>
       </c>
       <c r="G32" s="6"/>
-      <c r="H32" s="12"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
@@ -4389,7 +4375,7 @@
         <v>41</v>
       </c>
       <c r="G33" s="6"/>
-      <c r="H33" s="12" t="s">
+      <c r="H33" t="s">
         <v>126</v>
       </c>
       <c r="K33" s="6"/>
@@ -4403,7 +4389,6 @@
         <v>42</v>
       </c>
       <c r="G34" s="6"/>
-      <c r="H34" s="12"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
@@ -4415,7 +4400,7 @@
         <v>43</v>
       </c>
       <c r="G35" s="6"/>
-      <c r="H35" s="12" t="s">
+      <c r="H35" t="s">
         <v>158</v>
       </c>
       <c r="K35" s="6"/>
@@ -4429,7 +4414,7 @@
         <v>44</v>
       </c>
       <c r="G36" s="6"/>
-      <c r="H36" s="12" t="s">
+      <c r="H36" t="s">
         <v>158</v>
       </c>
       <c r="K36" s="6"/>
@@ -4443,7 +4428,7 @@
         <v>45</v>
       </c>
       <c r="G37" s="6"/>
-      <c r="H37" s="12" t="s">
+      <c r="H37" t="s">
         <v>158</v>
       </c>
       <c r="K37" s="6"/>
@@ -4457,7 +4442,7 @@
         <v>46</v>
       </c>
       <c r="G38" s="6"/>
-      <c r="H38" s="12" t="s">
+      <c r="H38" t="s">
         <v>158</v>
       </c>
       <c r="K38" s="6"/>
@@ -4471,7 +4456,7 @@
         <v>47</v>
       </c>
       <c r="G39" s="6"/>
-      <c r="H39" s="12" t="s">
+      <c r="H39" t="s">
         <v>158</v>
       </c>
       <c r="K39" s="6"/>
@@ -4485,7 +4470,7 @@
         <v>48</v>
       </c>
       <c r="G40" s="6"/>
-      <c r="H40" s="12" t="s">
+      <c r="H40" t="s">
         <v>158</v>
       </c>
       <c r="K40" s="6"/>
@@ -4499,7 +4484,7 @@
         <v>49</v>
       </c>
       <c r="G41" s="6"/>
-      <c r="H41" s="12" t="s">
+      <c r="H41" t="s">
         <v>158</v>
       </c>
       <c r="K41" s="6"/>
@@ -4513,7 +4498,7 @@
         <v>50</v>
       </c>
       <c r="G42" s="6"/>
-      <c r="H42" s="12" t="s">
+      <c r="H42" t="s">
         <v>149</v>
       </c>
       <c r="K42" s="6"/>
@@ -4527,7 +4512,6 @@
         <v>51</v>
       </c>
       <c r="G43" s="6"/>
-      <c r="H43" s="12"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
       <c r="M43" s="6"/>
@@ -4539,7 +4523,6 @@
         <v>52</v>
       </c>
       <c r="G44" s="6"/>
-      <c r="H44" s="12"/>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
@@ -4551,7 +4534,6 @@
         <v>53</v>
       </c>
       <c r="G45" s="6"/>
-      <c r="H45" s="12"/>
       <c r="K45" s="6"/>
       <c r="L45" s="6"/>
       <c r="M45" s="6"/>
@@ -4563,7 +4545,6 @@
         <v>54</v>
       </c>
       <c r="G46" s="6"/>
-      <c r="H46" s="12"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
       <c r="M46" s="6"/>
@@ -4575,7 +4556,6 @@
         <v>55</v>
       </c>
       <c r="G47" s="6"/>
-      <c r="H47" s="12"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
@@ -4587,7 +4567,7 @@
         <v>56</v>
       </c>
       <c r="G48" s="6"/>
-      <c r="H48" s="12" t="s">
+      <c r="H48" t="s">
         <v>153</v>
       </c>
       <c r="K48" s="6"/>
@@ -4601,7 +4581,6 @@
         <v>57</v>
       </c>
       <c r="G49" s="6"/>
-      <c r="H49" s="12"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
@@ -4613,7 +4592,6 @@
         <v>58</v>
       </c>
       <c r="G50" s="6"/>
-      <c r="H50" s="12"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
@@ -4625,7 +4603,6 @@
         <v>59</v>
       </c>
       <c r="G51" s="6"/>
-      <c r="H51" s="12"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
@@ -4637,7 +4614,6 @@
         <v>60</v>
       </c>
       <c r="G52" s="6"/>
-      <c r="H52" s="12"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
       <c r="M52" s="6"/>
@@ -4649,7 +4625,6 @@
         <v>61</v>
       </c>
       <c r="G53" s="6"/>
-      <c r="H53" s="12"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
       <c r="M53" s="6"/>
@@ -4661,7 +4636,6 @@
         <v>62</v>
       </c>
       <c r="G54" s="6"/>
-      <c r="H54" s="12"/>
       <c r="K54" s="6"/>
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
@@ -4673,7 +4647,6 @@
         <v>63</v>
       </c>
       <c r="G55" s="6"/>
-      <c r="H55" s="12"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
       <c r="M55" s="6"/>
@@ -4690,7 +4663,7 @@
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
-      <c r="H56" s="11"/>
+      <c r="H56" s="10"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
       <c r="K56" s="8"/>
@@ -4709,7 +4682,7 @@
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
-      <c r="H57" s="11"/>
+      <c r="H57" s="10"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
       <c r="K57" s="8"/>
@@ -4728,7 +4701,7 @@
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
-      <c r="H58" s="11"/>
+      <c r="H58" s="10"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
       <c r="K58" s="8"/>
@@ -4747,7 +4720,7 @@
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
-      <c r="H59" s="11"/>
+      <c r="H59" s="10"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
       <c r="K59" s="8"/>
@@ -4766,7 +4739,7 @@
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
-      <c r="H60" s="11"/>
+      <c r="H60" s="10"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
       <c r="K60" s="8"/>
@@ -4780,7 +4753,6 @@
         <v>64</v>
       </c>
       <c r="G61" s="6"/>
-      <c r="H61" s="12"/>
       <c r="K61" s="6"/>
       <c r="L61" s="6"/>
       <c r="M61" s="6"/>
@@ -4792,7 +4764,6 @@
         <v>65</v>
       </c>
       <c r="G62" s="6"/>
-      <c r="H62" s="12"/>
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
       <c r="M62" s="6"/>
@@ -4804,7 +4775,6 @@
         <v>66</v>
       </c>
       <c r="G63" s="6"/>
-      <c r="H63" s="12"/>
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
       <c r="M63" s="6"/>
@@ -4816,7 +4786,6 @@
         <v>67</v>
       </c>
       <c r="G64" s="6"/>
-      <c r="H64" s="12"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
       <c r="M64" s="6"/>
@@ -4828,7 +4797,6 @@
         <v>68</v>
       </c>
       <c r="G65" s="6"/>
-      <c r="H65" s="12"/>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
       <c r="M65" s="6"/>
@@ -4840,7 +4808,6 @@
         <v>69</v>
       </c>
       <c r="G66" s="6"/>
-      <c r="H66" s="12"/>
       <c r="K66" s="6"/>
       <c r="L66" s="6"/>
       <c r="M66" s="6"/>
@@ -4852,7 +4819,6 @@
         <v>70</v>
       </c>
       <c r="G67" s="6"/>
-      <c r="H67" s="12"/>
       <c r="K67" s="6"/>
       <c r="L67" s="6"/>
       <c r="M67" s="6"/>
@@ -4864,7 +4830,6 @@
         <v>71</v>
       </c>
       <c r="G68" s="6"/>
-      <c r="H68" s="12"/>
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
       <c r="M68" s="6"/>
@@ -4876,7 +4841,6 @@
         <v>72</v>
       </c>
       <c r="G69" s="6"/>
-      <c r="H69" s="12"/>
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="6"/>
@@ -4888,7 +4852,6 @@
         <v>73</v>
       </c>
       <c r="G70" s="6"/>
-      <c r="H70" s="12"/>
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
       <c r="M70" s="6"/>
@@ -4900,7 +4863,6 @@
         <v>74</v>
       </c>
       <c r="G71" s="6"/>
-      <c r="H71" s="12"/>
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
       <c r="M71" s="6"/>
@@ -4912,7 +4874,6 @@
         <v>75</v>
       </c>
       <c r="G72" s="6"/>
-      <c r="H72" s="12"/>
       <c r="K72" s="6"/>
       <c r="L72" s="6"/>
       <c r="M72" s="6"/>
@@ -4924,7 +4885,6 @@
         <v>76</v>
       </c>
       <c r="G73" s="6"/>
-      <c r="H73" s="12"/>
       <c r="K73" s="6"/>
       <c r="L73" s="6"/>
       <c r="M73" s="6"/>
@@ -4936,7 +4896,6 @@
         <v>77</v>
       </c>
       <c r="G74" s="6"/>
-      <c r="H74" s="12"/>
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
       <c r="M74" s="6"/>
@@ -4948,7 +4907,6 @@
         <v>78</v>
       </c>
       <c r="G75" s="6"/>
-      <c r="H75" s="12"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
@@ -4960,7 +4918,6 @@
         <v>79</v>
       </c>
       <c r="G76" s="6"/>
-      <c r="H76" s="12"/>
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
       <c r="M76" s="6"/>
@@ -4972,7 +4929,6 @@
         <v>80</v>
       </c>
       <c r="G77" s="6"/>
-      <c r="H77" s="12"/>
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
       <c r="M77" s="6"/>
@@ -4984,7 +4940,6 @@
         <v>81</v>
       </c>
       <c r="G78" s="6"/>
-      <c r="H78" s="12"/>
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
       <c r="M78" s="6"/>
@@ -4996,7 +4951,6 @@
         <v>82</v>
       </c>
       <c r="G79" s="6"/>
-      <c r="H79" s="12"/>
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
       <c r="M79" s="6"/>
@@ -5008,7 +4962,6 @@
         <v>83</v>
       </c>
       <c r="G80" s="6"/>
-      <c r="H80" s="12"/>
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
       <c r="M80" s="6"/>
@@ -5020,7 +4973,6 @@
         <v>84</v>
       </c>
       <c r="G81" s="6"/>
-      <c r="H81" s="12"/>
       <c r="K81" s="6"/>
       <c r="L81" s="6"/>
       <c r="M81" s="6"/>
@@ -5032,7 +4984,6 @@
         <v>85</v>
       </c>
       <c r="G82" s="6"/>
-      <c r="H82" s="12"/>
       <c r="K82" s="6"/>
       <c r="L82" s="6"/>
       <c r="M82" s="6"/>
@@ -5044,7 +4995,6 @@
         <v>85</v>
       </c>
       <c r="G83" s="6"/>
-      <c r="H83" s="12"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
       <c r="M83" s="6"/>
@@ -5056,7 +5006,6 @@
         <v>86</v>
       </c>
       <c r="G84" s="6"/>
-      <c r="H84" s="12"/>
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
       <c r="M84" s="6"/>
@@ -5068,7 +5017,6 @@
         <v>87</v>
       </c>
       <c r="G85" s="6"/>
-      <c r="H85" s="12"/>
       <c r="K85" s="6"/>
       <c r="L85" s="6"/>
       <c r="M85" s="6"/>
@@ -5080,7 +5028,6 @@
         <v>88</v>
       </c>
       <c r="G86" s="6"/>
-      <c r="H86" s="12"/>
       <c r="K86" s="6"/>
       <c r="L86" s="6"/>
       <c r="M86" s="6"/>
@@ -5092,7 +5039,6 @@
         <v>89</v>
       </c>
       <c r="G87" s="6"/>
-      <c r="H87" s="12"/>
       <c r="K87" s="6"/>
       <c r="L87" s="6"/>
       <c r="M87" s="6"/>
@@ -5104,7 +5050,6 @@
         <v>90</v>
       </c>
       <c r="G88" s="6"/>
-      <c r="H88" s="12"/>
       <c r="K88" s="6"/>
       <c r="L88" s="6"/>
       <c r="M88" s="6"/>
@@ -5116,7 +5061,6 @@
         <v>91</v>
       </c>
       <c r="G89" s="6"/>
-      <c r="H89" s="12"/>
       <c r="K89" s="6"/>
       <c r="L89" s="6"/>
       <c r="M89" s="6"/>
@@ -5128,7 +5072,6 @@
         <v>92</v>
       </c>
       <c r="G90" s="6"/>
-      <c r="H90" s="12"/>
       <c r="K90" s="6"/>
       <c r="L90" s="6"/>
       <c r="M90" s="6"/>
@@ -5140,7 +5083,6 @@
         <v>93</v>
       </c>
       <c r="G91" s="6"/>
-      <c r="H91" s="12"/>
       <c r="K91" s="6"/>
       <c r="L91" s="6"/>
       <c r="M91" s="6"/>
@@ -5152,7 +5094,6 @@
         <v>94</v>
       </c>
       <c r="G92" s="6"/>
-      <c r="H92" s="12"/>
       <c r="K92" s="6"/>
       <c r="L92" s="6"/>
       <c r="M92" s="6"/>
@@ -5164,7 +5105,6 @@
         <v>95</v>
       </c>
       <c r="G93" s="6"/>
-      <c r="H93" s="12"/>
       <c r="K93" s="6"/>
       <c r="L93" s="6"/>
       <c r="M93" s="6"/>
@@ -5176,7 +5116,6 @@
         <v>96</v>
       </c>
       <c r="G94" s="6"/>
-      <c r="H94" s="12"/>
       <c r="K94" s="6"/>
       <c r="L94" s="6"/>
       <c r="M94" s="6"/>
@@ -5188,7 +5127,6 @@
         <v>97</v>
       </c>
       <c r="G95" s="6"/>
-      <c r="H95" s="12"/>
       <c r="K95" s="6"/>
       <c r="L95" s="6"/>
       <c r="M95" s="6"/>
@@ -5200,7 +5138,6 @@
         <v>97</v>
       </c>
       <c r="G96" s="6"/>
-      <c r="H96" s="12"/>
       <c r="K96" s="6"/>
       <c r="L96" s="6"/>
       <c r="M96" s="6"/>
@@ -5212,7 +5149,6 @@
         <v>97</v>
       </c>
       <c r="G97" s="6"/>
-      <c r="H97" s="12"/>
       <c r="K97" s="6"/>
       <c r="L97" s="6"/>
       <c r="M97" s="6"/>
@@ -5224,7 +5160,6 @@
         <v>98</v>
       </c>
       <c r="G98" s="6"/>
-      <c r="H98" s="12"/>
       <c r="K98" s="6"/>
       <c r="L98" s="6"/>
       <c r="M98" s="6"/>
@@ -5236,7 +5171,6 @@
         <v>99</v>
       </c>
       <c r="G99" s="6"/>
-      <c r="H99" s="12"/>
       <c r="K99" s="6"/>
       <c r="L99" s="6"/>
       <c r="M99" s="6"/>
@@ -5248,7 +5182,6 @@
         <v>100</v>
       </c>
       <c r="G100" s="6"/>
-      <c r="H100" s="12"/>
       <c r="K100" s="6"/>
       <c r="L100" s="6"/>
       <c r="M100" s="6"/>
@@ -5260,7 +5193,6 @@
         <v>101</v>
       </c>
       <c r="G101" s="6"/>
-      <c r="H101" s="12"/>
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
       <c r="M101" s="6"/>
@@ -5272,7 +5204,6 @@
         <v>102</v>
       </c>
       <c r="G102" s="6"/>
-      <c r="H102" s="12"/>
       <c r="K102" s="6"/>
       <c r="L102" s="6"/>
       <c r="M102" s="6"/>
@@ -5284,7 +5215,6 @@
         <v>103</v>
       </c>
       <c r="G103" s="6"/>
-      <c r="H103" s="12"/>
       <c r="K103" s="6"/>
       <c r="L103" s="6"/>
       <c r="M103" s="6"/>
@@ -5296,7 +5226,6 @@
         <v>104</v>
       </c>
       <c r="G104" s="6"/>
-      <c r="H104" s="12"/>
       <c r="K104" s="6"/>
       <c r="L104" s="6"/>
       <c r="M104" s="6"/>
@@ -5308,7 +5237,6 @@
         <v>105</v>
       </c>
       <c r="G105" s="6"/>
-      <c r="H105" s="12"/>
       <c r="K105" s="6"/>
       <c r="L105" s="6"/>
       <c r="M105" s="6"/>
@@ -5320,7 +5248,6 @@
         <v>106</v>
       </c>
       <c r="G106" s="6"/>
-      <c r="H106" s="12"/>
       <c r="K106" s="6"/>
       <c r="L106" s="6"/>
       <c r="M106" s="6"/>
@@ -5332,7 +5259,6 @@
         <v>107</v>
       </c>
       <c r="G107" s="6"/>
-      <c r="H107" s="12"/>
       <c r="K107" s="6"/>
       <c r="L107" s="6"/>
       <c r="M107" s="6"/>
@@ -5344,7 +5270,6 @@
         <v>108</v>
       </c>
       <c r="G108" s="6"/>
-      <c r="H108" s="12"/>
       <c r="K108" s="6"/>
       <c r="L108" s="6"/>
       <c r="M108" s="6"/>
@@ -5356,7 +5281,6 @@
         <v>109</v>
       </c>
       <c r="G109" s="6"/>
-      <c r="H109" s="12"/>
       <c r="K109" s="6"/>
       <c r="L109" s="6"/>
       <c r="M109" s="6"/>
@@ -5368,7 +5292,6 @@
         <v>110</v>
       </c>
       <c r="G110" s="6"/>
-      <c r="H110" s="12"/>
       <c r="K110" s="6"/>
       <c r="L110" s="6"/>
       <c r="M110" s="6"/>
@@ -5380,7 +5303,6 @@
         <v>111</v>
       </c>
       <c r="G111" s="6"/>
-      <c r="H111" s="12"/>
       <c r="K111" s="6"/>
       <c r="L111" s="6"/>
       <c r="M111" s="6"/>
@@ -5392,7 +5314,6 @@
         <v>112</v>
       </c>
       <c r="G112" s="6"/>
-      <c r="H112" s="12"/>
       <c r="K112" s="6"/>
       <c r="L112" s="6"/>
       <c r="M112" s="6"/>
@@ -5404,7 +5325,6 @@
         <v>113</v>
       </c>
       <c r="G113" s="6"/>
-      <c r="H113" s="12"/>
       <c r="K113" s="6"/>
       <c r="L113" s="6"/>
       <c r="M113" s="6"/>
@@ -5416,7 +5336,6 @@
         <v>114</v>
       </c>
       <c r="G114" s="6"/>
-      <c r="H114" s="12"/>
       <c r="K114" s="6"/>
       <c r="L114" s="6"/>
       <c r="M114" s="6"/>
@@ -5428,7 +5347,6 @@
         <v>115</v>
       </c>
       <c r="G115" s="6"/>
-      <c r="H115" s="12"/>
       <c r="K115" s="6"/>
       <c r="L115" s="6"/>
       <c r="M115" s="6"/>
@@ -5440,7 +5358,6 @@
         <v>116</v>
       </c>
       <c r="G116" s="6"/>
-      <c r="H116" s="12"/>
       <c r="K116" s="6"/>
       <c r="L116" s="6"/>
       <c r="M116" s="6"/>
@@ -5468,4 +5385,1844 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8CCFB3-69A9-46C7-BF8F-BFEC7559D5C6}">
+  <dimension ref="A1:M117"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" activeCellId="5" sqref="A4:M4 A15:M15 A16:M16 A17:M17 A19:M19 A23:M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="102" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="102" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="22" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[Block of Hours - Actual Rates]-STANDARD</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[Block of Hours - Blended Rates]-STANDARD</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="12" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>--[]-</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[Time &amp; Materials]-STANDARD</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[Upfront (Annual)]-STANDARD</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-HYBRID-[Change Order]-STANDARD</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>GOV-NRR-[GCC High Licenses - Add On Orders]-STANDARD</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>GOV-NRR-[GCC High Licenses - Contract Addendum]-STANDARD</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>GOV-NRR-[Block of Hours - Actual Rates]-STANDARD</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>GOV-NRR-[Block of Hours - Blended Rates]-STANDARD</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>GOV-NRR-[Non-Recurring]-STANDARD</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>GOV-NRR-[Non-Recurring - Legacy Bronze]-STANDARD</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>GOV-NRR-[Renewal]-STANDARD</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="12" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>--[]-</v>
+      </c>
+      <c r="J15" s="14"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="12" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>--[]-</v>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="12" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>--[]-</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[Non-Recurring]-STANDARD</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="14"/>
+      <c r="I19" s="12" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>--[]-</v>
+      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[OHD Master Quotes]-CLIENT</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[Physical Security]-STANDARD</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[Firewall End of Service Renewal]-USER-JSobernheim</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="12" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>--[]-</v>
+      </c>
+      <c r="J23" s="14"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>MPC-NRR-[Renewal]-STANDARD</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>RIT-NRR-[Security Risk Assessment]-STANDARD</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>VMS-NRR-[Fixed Labor Rates]-</v>
+      </c>
+      <c r="J26" s="9"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>VMS-NRR-[PSP Labor Rates]-</v>
+      </c>
+      <c r="J27" s="9"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f>_xlfn.CONCAT(Table432[[#This Row],[Company ID]], "-", Table432[[#This Row],[Category]], "-[", Table432[[#This Row],[Template Description]], "]-", IF(Table432[[#This Row],[Type]]="USER", _xlfn.CONCAT(Table432[[#This Row],[Type]], "-", Table432[[#This Row],[ModifiedBy]]), Table432[[#This Row],[Type]]))</f>
+        <v>VMS-NRR-[Renewal]-</v>
+      </c>
+      <c r="J28" s="9"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="H32" t="s">
+        <v>135</v>
+      </c>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="6"/>
+      <c r="H34" t="s">
+        <v>126</v>
+      </c>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" t="s">
+        <v>158</v>
+      </c>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" t="s">
+        <v>158</v>
+      </c>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" t="s">
+        <v>158</v>
+      </c>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" t="s">
+        <v>158</v>
+      </c>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" t="s">
+        <v>158</v>
+      </c>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="H41" t="s">
+        <v>158</v>
+      </c>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="6"/>
+      <c r="H42" t="s">
+        <v>158</v>
+      </c>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="6"/>
+      <c r="H43" t="s">
+        <v>149</v>
+      </c>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" t="s">
+        <v>153</v>
+      </c>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="G51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="G52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="G53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="G54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="G56" s="6"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="8"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="7"/>
+      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="8"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="8"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="8"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="8"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+      <c r="G62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="G63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="G64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>67</v>
+      </c>
+      <c r="G65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>68</v>
+      </c>
+      <c r="G66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>69</v>
+      </c>
+      <c r="G67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>70</v>
+      </c>
+      <c r="G68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+      <c r="G69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="6"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>72</v>
+      </c>
+      <c r="G70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="6"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>73</v>
+      </c>
+      <c r="G71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="6"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>74</v>
+      </c>
+      <c r="G72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="6"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>75</v>
+      </c>
+      <c r="G73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="6"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>76</v>
+      </c>
+      <c r="G74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>77</v>
+      </c>
+      <c r="G75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="6"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>78</v>
+      </c>
+      <c r="G76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+      <c r="G77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>80</v>
+      </c>
+      <c r="G78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>81</v>
+      </c>
+      <c r="G79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>82</v>
+      </c>
+      <c r="G80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>83</v>
+      </c>
+      <c r="G81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>84</v>
+      </c>
+      <c r="G82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>85</v>
+      </c>
+      <c r="G83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="G84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="G86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="G87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="G88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="6"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="G89" s="6"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="6"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="G90" s="6"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="6"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="G91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="6"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="G92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="6"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+      <c r="G93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="G94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>96</v>
+      </c>
+      <c r="G95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+      <c r="G96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>97</v>
+      </c>
+      <c r="G97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
+      <c r="M97" s="6"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="G98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="G99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="G100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="G101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6"/>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="G102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="G103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="G104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="6"/>
+      <c r="M104" s="6"/>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="G105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+      <c r="G106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+      <c r="G107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="6"/>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+      <c r="G108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+      <c r="G109" s="6"/>
+      <c r="K109" s="6"/>
+      <c r="L109" s="6"/>
+      <c r="M109" s="6"/>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+      <c r="G110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
+      <c r="M110" s="6"/>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+      <c r="G111" s="6"/>
+      <c r="K111" s="6"/>
+      <c r="L111" s="6"/>
+      <c r="M111" s="6"/>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+      <c r="G112" s="6"/>
+      <c r="K112" s="6"/>
+      <c r="L112" s="6"/>
+      <c r="M112" s="6"/>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="G113" s="6"/>
+      <c r="K113" s="6"/>
+      <c r="L113" s="6"/>
+      <c r="M113" s="6"/>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+      <c r="G114" s="6"/>
+      <c r="K114" s="6"/>
+      <c r="L114" s="6"/>
+      <c r="M114" s="6"/>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+      <c r="G115" s="6"/>
+      <c r="K115" s="6"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="6"/>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+      <c r="G116" s="6"/>
+      <c r="K116" s="6"/>
+      <c r="L116" s="6"/>
+      <c r="M116" s="6"/>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="G117" s="6"/>
+      <c r="K117" s="6"/>
+      <c r="L117" s="6"/>
+      <c r="M117" s="6"/>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J30:J117 G2:G21 G22:G117 K2:M21 K22:M117" xr:uid="{A27EE379-DB89-4EA9-B79F-4B27139B69A3}">
+      <formula1>"Keep, Delete, Modify, Merge, TBD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21 C22:C117" xr:uid="{EBA950E6-377D-4726-95F4-22A954FA5625}">
+      <formula1>"NRR, MRR, HYBRID"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21 E22:E117" xr:uid="{4E48B32E-B44A-4444-8D54-F4D203FA182E}">
+      <formula1>"STANDARD, USER, CLIENT"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B117" xr:uid="{8DB02A32-4654-4A9C-A1A0-4D21ECFABBED}">
+      <formula1>"MPC, F1, VMS, RIT, SSI, GOV"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>